<commit_message>
small changes in the Excel writer
</commit_message>
<xml_diff>
--- a/results/excel/accuracy_score.xlsx
+++ b/results/excel/accuracy_score.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
   <si>
     <t>Classification results: accuracy score</t>
   </si>
@@ -25,7 +25,7 @@
     <t>General information about the classification software</t>
   </si>
   <si>
-    <t>Issue date: 26/11/2020 11:15:44</t>
+    <t>Issue date: 26/11/2020 20:45:51</t>
   </si>
   <si>
     <t>Python version: Python 3.7.6</t>
@@ -97,6 +97,18 @@
     <t>57.09</t>
   </si>
   <si>
+    <t>Stylistic Features: fdf, mef, e50th, frc</t>
+  </si>
+  <si>
+    <t>lowercase</t>
+  </si>
+  <si>
+    <t>5 folds X 20 iterations CV</t>
+  </si>
+  <si>
+    <t>86.1</t>
+  </si>
+  <si>
     <t>Number</t>
   </si>
   <si>
@@ -115,26 +127,26 @@
     <t>Technique</t>
   </si>
   <si>
-    <t>MLPClassifier</t>
-  </si>
-  <si>
-    <t>LinearSVC</t>
-  </si>
-  <si>
-    <t>LogisticRegression</t>
-  </si>
-  <si>
-    <t>RandomForest</t>
-  </si>
-  <si>
-    <t>MultinomialNB</t>
+    <t>MLP</t>
+  </si>
+  <si>
+    <t>SVC</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>MNB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,53 +159,52 @@
       <u/>
       <sz val="17"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -216,19 +227,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -241,8 +253,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:K18" totalsRowShown="0">
-  <autoFilter ref="A15:K18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:K19" totalsRowShown="0">
+  <autoFilter ref="A15:K19"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Number"/>
     <tableColumn id="2" name="Language"/>
@@ -250,13 +262,13 @@
     <tableColumn id="4" name="Features selectors"/>
     <tableColumn id="5" name="Pre-processing"/>
     <tableColumn id="6" name="Technique"/>
-    <tableColumn id="7" name="MLPClassifier"/>
-    <tableColumn id="8" name="LinearSVC"/>
-    <tableColumn id="9" name="LogisticRegression"/>
-    <tableColumn id="10" name="RandomForest"/>
-    <tableColumn id="11" name="MultinomialNB"/>
+    <tableColumn id="7" name="MLP"/>
+    <tableColumn id="8" name="SVC"/>
+    <tableColumn id="9" name="LR"/>
+    <tableColumn id="10" name="RF"/>
+    <tableColumn id="11" name="MNB"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -545,17 +557,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -564,191 +576,214 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" t="s">
+        <v>39</v>
+      </c>
+      <c r="J15" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="8">
+        <v>800</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="8">
+        <v>80</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="8">
+        <v>80</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="8">
+        <v>209</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D19" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C15" t="s">
+      <c r="F19" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D15" t="s">
+      <c r="J19" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="E15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" t="s">
-        <v>35</v>
-      </c>
-      <c r="J15" t="s">
-        <v>36</v>
-      </c>
-      <c r="K15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="7">
-        <v>800</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="7">
-        <v>80</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="7">
-        <v>80</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor doc2vectransfomer and add word2vectransfomer
</commit_message>
<xml_diff>
--- a/results/excel/accuracy_score.xlsx
+++ b/results/excel/accuracy_score.xlsx
@@ -25,7 +25,7 @@
     <t>General information about the classification software</t>
   </si>
   <si>
-    <t>Issue date: 01/12/2020 18:03:20</t>
+    <t>Issue date: 02/12/2020 12:20:32</t>
   </si>
   <si>
     <t>Python version: Python 3.7.3</t>
@@ -79,16 +79,16 @@
     <t>5 folds X 20 iterations CV</t>
   </si>
   <si>
-    <t>63.43*</t>
-  </si>
-  <si>
-    <t>63.58*</t>
-  </si>
-  <si>
-    <t>63.38*</t>
-  </si>
-  <si>
-    <t>58.75*</t>
+    <t>65.03*</t>
+  </si>
+  <si>
+    <t>64.85*</t>
+  </si>
+  <si>
+    <t>63.25*</t>
+  </si>
+  <si>
+    <t>64.8*</t>
   </si>
   <si>
     <t>Number</t>
@@ -688,10 +688,10 @@
       <c r="F17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I17" s="5" t="s">

</xml_diff>

<commit_message>
Write to xlsx fixed
</commit_message>
<xml_diff>
--- a/results/excel/accuracy_score.xlsx
+++ b/results/excel/accuracy_score.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>Classification results: accuracy score</t>
   </si>
@@ -25,10 +25,10 @@
     <t>General information about the classification software</t>
   </si>
   <si>
-    <t>Issue date: 02/12/2020 12:20:32</t>
-  </si>
-  <si>
-    <t>Python version: Python 3.7.3</t>
+    <t>Issue date: 03/12/2020 11:42:50</t>
+  </si>
+  <si>
+    <t>Python version: Python 3.7.6</t>
   </si>
   <si>
     <t>Python classification libraries: keras, sklearn, tensorflow, VADAR from nltk, WordCloud</t>
@@ -79,16 +79,28 @@
     <t>5 folds X 20 iterations CV</t>
   </si>
   <si>
-    <t>65.03*</t>
-  </si>
-  <si>
-    <t>64.85*</t>
-  </si>
-  <si>
-    <t>63.25*</t>
-  </si>
-  <si>
-    <t>64.8*</t>
+    <t>64.3*</t>
+  </si>
+  <si>
+    <t>65.3*</t>
+  </si>
+  <si>
+    <t>65.65*</t>
+  </si>
+  <si>
+    <t>64.92*</t>
+  </si>
+  <si>
+    <t>62.98*</t>
+  </si>
+  <si>
+    <t>62.4*</t>
+  </si>
+  <si>
+    <t>61.83*</t>
+  </si>
+  <si>
+    <t>59.4*</t>
   </si>
   <si>
     <t>Number</t>
@@ -235,8 +247,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:K17" totalsRowShown="0">
-  <autoFilter ref="A15:K17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:K18" totalsRowShown="0">
+  <autoFilter ref="A15:K18"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Number"/>
     <tableColumn id="2" name="Language"/>
@@ -250,7 +262,7 @@
     <tableColumn id="10" name="RF"/>
     <tableColumn id="11" name="MNB"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -539,7 +551,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -613,37 +625,37 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G15" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H15" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="I15" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="J15" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="K15" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -669,7 +681,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:10">
       <c r="A17" s="8">
         <v>0</v>
       </c>
@@ -688,20 +700,49 @@
       <c r="F17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="5" t="s">
         <v>21</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K17" s="5" t="s">
-        <v>18</v>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="8">
+        <v>0</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add option to configure a range of files at once
</commit_message>
<xml_diff>
--- a/results/excel/accuracy_score.xlsx
+++ b/results/excel/accuracy_score.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>Classification results: accuracy score</t>
   </si>
@@ -25,10 +25,10 @@
     <t>General information about the classification software</t>
   </si>
   <si>
-    <t>Issue date: 03/12/2020 11:42:50</t>
-  </si>
-  <si>
-    <t>Python version: Python 3.7.6</t>
+    <t>Issue date: 03/12/2020 11:53:13</t>
+  </si>
+  <si>
+    <t>Python version: Python 3.7.3</t>
   </si>
   <si>
     <t>Python classification libraries: keras, sklearn, tensorflow, VADAR from nltk, WordCloud</t>
@@ -73,22 +73,25 @@
     <t>nan</t>
   </si>
   <si>
+    <t>Word2VecTransfomer</t>
+  </si>
+  <si>
+    <t>5 folds X 20 iterations CV</t>
+  </si>
+  <si>
+    <t>70.1*</t>
+  </si>
+  <si>
+    <t>68.68*</t>
+  </si>
+  <si>
+    <t>62.65*</t>
+  </si>
+  <si>
+    <t>72.32*</t>
+  </si>
+  <si>
     <t>Doc2VecTransfomer</t>
-  </si>
-  <si>
-    <t>5 folds X 20 iterations CV</t>
-  </si>
-  <si>
-    <t>64.3*</t>
-  </si>
-  <si>
-    <t>65.3*</t>
-  </si>
-  <si>
-    <t>65.65*</t>
-  </si>
-  <si>
-    <t>64.92*</t>
   </si>
   <si>
     <t>62.98*</t>
@@ -558,7 +561,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="26.7109375" customWidth="1"/>
@@ -625,37 +628,37 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -695,7 +698,7 @@
         <v>15</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>20</v>
@@ -706,10 +709,10 @@
       <c r="H17" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="J17" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -721,7 +724,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>15</v>
@@ -733,16 +736,16 @@
         <v>20</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Split baseline by the language
</commit_message>
<xml_diff>
--- a/results/excel/accuracy_score.xlsx
+++ b/results/excel/accuracy_score.xlsx
@@ -25,10 +25,10 @@
     <t>General information about the classification software</t>
   </si>
   <si>
-    <t>Issue date: 07/12/2020 12:34:44</t>
-  </si>
-  <si>
-    <t>Python version: Python 3.7.3</t>
+    <t>Issue date: 10/12/2020 11:27:59</t>
+  </si>
+  <si>
+    <t>Python version: Python 3.7.6</t>
   </si>
   <si>
     <t>Python classification libraries: keras, sklearn, tensorflow, VADAR from nltk, WordCloud</t>
@@ -265,7 +265,7 @@
     <tableColumn id="10" name="RF"/>
     <tableColumn id="11" name="MNB"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 

</xml_diff>

<commit_message>
features selection display in the Excel fixed
</commit_message>
<xml_diff>
--- a/results/excel/accuracy_score.xlsx
+++ b/results/excel/accuracy_score.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t>Classification results: accuracy score</t>
   </si>
@@ -25,10 +25,10 @@
     <t>General information about the classification software</t>
   </si>
   <si>
-    <t>Issue date: 10/12/2020 11:27:59</t>
-  </si>
-  <si>
-    <t>Python version: Python 3.7.6</t>
+    <t>Issue date: 21/12/2020 11:37:48</t>
+  </si>
+  <si>
+    <t>Python version: Python 3.8.5</t>
   </si>
   <si>
     <t>Python classification libraries: keras, sklearn, tensorflow, VADAR from nltk, WordCloud</t>
@@ -89,6 +89,16 @@
   </si>
   <si>
     <t>72.32*</t>
+  </si>
+  <si>
+    <t>TF: 100 words unigrams
+Stylistic Features: cc</t>
+  </si>
+  <si>
+    <t>chi2</t>
+  </si>
+  <si>
+    <t>stemming</t>
   </si>
   <si>
     <t>Doc2VecTransfomer</t>
@@ -250,8 +260,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:K18" totalsRowShown="0">
-  <autoFilter ref="A15:K18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:K19" totalsRowShown="0">
+  <autoFilter ref="A15:K19"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Number"/>
     <tableColumn id="2" name="Language"/>
@@ -265,7 +275,7 @@
     <tableColumn id="10" name="RF"/>
     <tableColumn id="11" name="MNB"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -554,14 +564,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="26.7109375" customWidth="1"/>
@@ -628,37 +638,37 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G15" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I15" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="J15" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K15" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -684,7 +694,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:11">
       <c r="A17" s="8">
         <v>0</v>
       </c>
@@ -716,9 +726,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:11">
       <c r="A18" s="8">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>13</v>
@@ -727,25 +737,60 @@
         <v>25</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>20</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="I18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="8">
+        <v>0</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="D19" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="8" t="s">
         <v>29</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Problem the result writing fixed
</commit_message>
<xml_diff>
--- a/results/excel/accuracy_score.xlsx
+++ b/results/excel/accuracy_score.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Classification results: accuracy score</t>
   </si>
@@ -25,7 +25,7 @@
     <t>General information about the classification software</t>
   </si>
   <si>
-    <t>Issue date: 21/12/2020 11:37:48</t>
+    <t>Issue date: 22/12/2020 10:37:21</t>
   </si>
   <si>
     <t>Python version: Python 3.8.5</t>
@@ -55,65 +55,28 @@
     <t>Results:</t>
   </si>
   <si>
-    <t>English</t>
+    <t>Hebrew</t>
+  </si>
+  <si>
+    <t>Stylistic Features: acf,  aof,  caf,  e50th,  fdf,  frc,  huf,  mef,  vof</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>lowercase</t>
+  </si>
+  <si>
+    <t>5 folds X 20 iterations CV</t>
+  </si>
+  <si>
+    <t>51.5*</t>
   </si>
   <si>
     <t>BertTransformer</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>lowercase</t>
-  </si>
-  <si>
-    <t>5 folds X 1 iterations CV</t>
-  </si>
-  <si>
     <t>nan</t>
-  </si>
-  <si>
-    <t>Word2VecTransfomer</t>
-  </si>
-  <si>
-    <t>5 folds X 20 iterations CV</t>
-  </si>
-  <si>
-    <t>70.1*</t>
-  </si>
-  <si>
-    <t>68.68*</t>
-  </si>
-  <si>
-    <t>62.65*</t>
-  </si>
-  <si>
-    <t>72.32*</t>
-  </si>
-  <si>
-    <t>TF: 100 words unigrams
-Stylistic Features: cc</t>
-  </si>
-  <si>
-    <t>chi2</t>
-  </si>
-  <si>
-    <t>stemming</t>
-  </si>
-  <si>
-    <t>Doc2VecTransfomer</t>
-  </si>
-  <si>
-    <t>62.98*</t>
-  </si>
-  <si>
-    <t>62.4*</t>
-  </si>
-  <si>
-    <t>61.83*</t>
-  </si>
-  <si>
-    <t>59.4*</t>
   </si>
   <si>
     <t>Number</t>
@@ -260,8 +223,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:K19" totalsRowShown="0">
-  <autoFilter ref="A15:K19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:K17" totalsRowShown="0">
+  <autoFilter ref="A15:K17"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Number"/>
     <tableColumn id="2" name="Language"/>
@@ -275,7 +238,7 @@
     <tableColumn id="10" name="RF"/>
     <tableColumn id="11" name="MNB"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -564,14 +527,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="73.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="26.7109375" customWidth="1"/>
@@ -638,37 +601,37 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G15" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="H15" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="I15" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="J15" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="K15" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -690,11 +653,11 @@
       <c r="F16" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="H16" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:7">
       <c r="A17" s="8">
         <v>0</v>
       </c>
@@ -708,89 +671,13 @@
         <v>15</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F17" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="8">
-        <v>100</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="8">
-        <v>0</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add configs files for the 13 best families
</commit_message>
<xml_diff>
--- a/results/excel/accuracy_score.xlsx
+++ b/results/excel/accuracy_score.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natan\PycharmProjects\TextClassification2\results\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E42572B-9E65-4172-A31A-F101E93B6272}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>Classification results: accuracy score</t>
   </si>
@@ -25,7 +31,7 @@
     <t>General information about the classification software</t>
   </si>
   <si>
-    <t>Issue date: 29/12/2020 12:41:47</t>
+    <t>Issue date: 30/12/2020 11:56:12</t>
   </si>
   <si>
     <t>Python version: Python 3.7.6</t>
@@ -55,21 +61,60 @@
     <t>Results:</t>
   </si>
   <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>TF: 100 words unigrams</t>
+    <t>Hebrew</t>
   </si>
   <si>
     <t>None</t>
   </si>
   <si>
+    <t>lowercase</t>
+  </si>
+  <si>
     <t>5 folds X 20 iterations CV</t>
   </si>
   <si>
+    <t>52.33*</t>
+  </si>
+  <si>
+    <t>52.5*</t>
+  </si>
+  <si>
+    <t>61.25*</t>
+  </si>
+  <si>
     <t>50.0*</t>
   </si>
   <si>
+    <t>52.75*</t>
+  </si>
+  <si>
+    <t>53.5*</t>
+  </si>
+  <si>
+    <t>55.5*</t>
+  </si>
+  <si>
+    <t>55.47*</t>
+  </si>
+  <si>
+    <t>52.0*</t>
+  </si>
+  <si>
+    <t>55.23*</t>
+  </si>
+  <si>
+    <t>58.5*</t>
+  </si>
+  <si>
+    <t>57.5*</t>
+  </si>
+  <si>
+    <t>62.02*</t>
+  </si>
+  <si>
+    <t>51.0*</t>
+  </si>
+  <si>
     <t>Number</t>
   </si>
   <si>
@@ -103,18 +148,24 @@
     <t>MNB</t>
   </si>
   <si>
-    <t>RNN</t>
+    <t>Stylistic Features: negative</t>
+  </si>
+  <si>
+    <t>Stylistic Features: positive</t>
+  </si>
+  <si>
+    <t>Stylistic Features: positive, negative</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -124,51 +175,59 @@
       <sz val="17"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-      <family val="2"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-      <family val="2"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF808080"/>
       <name val="Times New Roman"/>
-      <family val="2"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF808080"/>
       <name val="Times New Roman"/>
-      <family val="2"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
-      <family val="2"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
-      <family val="2"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-      <family val="2"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-      <family val="2"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -191,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -201,44 +260,198 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:L16" totalsRowShown="0">
-  <autoFilter ref="A15:L16"/>
-  <tableColumns count="12">
-    <tableColumn id="1" name="Number"/>
-    <tableColumn id="2" name="Language"/>
-    <tableColumn id="3" name="Features types"/>
-    <tableColumn id="4" name="Features selectors"/>
-    <tableColumn id="5" name="Pre-processing"/>
-    <tableColumn id="6" name="Technique"/>
-    <tableColumn id="7" name="MLP"/>
-    <tableColumn id="8" name="SVC"/>
-    <tableColumn id="9" name="LR"/>
-    <tableColumn id="10" name="RF"/>
-    <tableColumn id="11" name="MNB"/>
-    <tableColumn id="12" name="RNN"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A15:K18" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A15:K18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Number" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Language" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Features types" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Features selectors" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Pre-processing" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Technique" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="MLP" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="SVC" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="LR" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="RF" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="MNB" dataDxfId="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -280,7 +493,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -312,9 +525,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -346,6 +577,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -521,51 +770,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.796875" style="2"/>
+    <col min="2" max="2" width="8.69921875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="30.69921875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.69921875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.69921875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26.69921875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -573,7 +824,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -581,7 +832,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -589,61 +840,58 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:11" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" t="s">
-        <v>24</v>
-      </c>
-      <c r="H15" t="s">
-        <v>25</v>
-      </c>
-      <c r="I15" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" t="s">
-        <v>27</v>
-      </c>
-      <c r="K15" t="s">
-        <v>28</v>
-      </c>
-      <c r="L15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+    <row r="15" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <v>0</v>
+        <v>3560</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>15</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>15</v>
@@ -651,14 +899,97 @@
       <c r="F16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="8" t="s">
         <v>17</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>3330</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>6890</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Another desperate attempt for BERT
</commit_message>
<xml_diff>
--- a/results/excel/accuracy_score.xlsx
+++ b/results/excel/accuracy_score.xlsx
@@ -25,7 +25,7 @@
     <t>General information about the classification software</t>
   </si>
   <si>
-    <t>Issue date: 17/01/2021 16:57:15</t>
+    <t>Issue date: 04/02/2021 19:30:44</t>
   </si>
   <si>
     <t>Python version: Python 3.7.6</t>
@@ -260,7 +260,7 @@
     <tableColumn id="11" name="MNB"/>
     <tableColumn id="12" name="RNN"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 

</xml_diff>

<commit_message>
Small bugs fixed in n_word_in_post
</commit_message>
<xml_diff>
--- a/results/excel/accuracy_score.xlsx
+++ b/results/excel/accuracy_score.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Classification results: accuracy score</t>
   </si>
@@ -25,10 +25,10 @@
     <t>General information about the classification software</t>
   </si>
   <si>
-    <t>Issue date: 04/02/2021 19:30:44</t>
-  </si>
-  <si>
-    <t>Python version: Python 3.7.6</t>
+    <t>Issue date: 14/01/2021 16:03:45</t>
+  </si>
+  <si>
+    <t>Python version: Python 3.8.5</t>
   </si>
   <si>
     <t>Python classification libraries: keras, sklearn, tensorflow, VADAR from nltk, WordCloud</t>
@@ -58,7 +58,7 @@
     <t>Hebrew</t>
   </si>
   <si>
-    <t>Stylistic Features: owc</t>
+    <t>Stylistic Features: vof, huf, aof, pnf, anf, agf, frc, mef, acf, fdf</t>
   </si>
   <si>
     <t>None</t>
@@ -67,34 +67,10 @@
     <t>lowercase</t>
   </si>
   <si>
-    <t>5 folds X 1 iterations CV</t>
-  </si>
-  <si>
-    <t>50.0*</t>
-  </si>
-  <si>
-    <t>Stylistic Features: frc, vof, aof, mef, caf, huf, anf, pnf, wef</t>
-  </si>
-  <si>
     <t>5 folds X 20 iterations CV</t>
   </si>
   <si>
-    <t>84.05</t>
-  </si>
-  <si>
-    <t>Stylistic Features: frc, vof, aof, mef, caf, huf, anf, agf, wef</t>
-  </si>
-  <si>
-    <t>Stylistic Features: frc, vof, aof, mef, caf, huf, pw, nw, pnf</t>
-  </si>
-  <si>
-    <t>82.38</t>
-  </si>
-  <si>
-    <t>Stylistic Features: frc, vof, aof, mef, caf, huf, pw, nw, agf</t>
-  </si>
-  <si>
-    <t>83.2</t>
+    <t>90.15V</t>
   </si>
   <si>
     <t>Number</t>
@@ -244,8 +220,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:L20" totalsRowShown="0">
-  <autoFilter ref="A15:L20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:L16" totalsRowShown="0">
+  <autoFilter ref="A15:L16"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Number"/>
     <tableColumn id="2" name="Language"/>
@@ -260,7 +236,7 @@
     <tableColumn id="11" name="MNB"/>
     <tableColumn id="12" name="RNN"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -549,14 +525,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="63.7109375" customWidth="1"/>
+    <col min="3" max="3" width="68.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="26.7109375" customWidth="1"/>
@@ -623,45 +599,45 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" t="s">
         <v>27</v>
       </c>
-      <c r="B15" t="s">
+      <c r="J15" t="s">
         <v>28</v>
       </c>
-      <c r="C15" t="s">
+      <c r="K15" t="s">
         <v>29</v>
       </c>
-      <c r="D15" t="s">
+      <c r="L15" t="s">
         <v>30</v>
-      </c>
-      <c r="E15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" t="s">
-        <v>35</v>
-      </c>
-      <c r="J15" t="s">
-        <v>36</v>
-      </c>
-      <c r="K15" t="s">
-        <v>37</v>
-      </c>
-      <c r="L15" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="8">
-        <v>1</v>
+        <v>1001</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>13</v>
@@ -678,100 +654,8 @@
       <c r="F16" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J16" s="6" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="8">
-        <v>666</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="8">
-        <v>665</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="8">
-        <v>933</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="8">
-        <v>932</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Few bug in the RNN fixed
</commit_message>
<xml_diff>
--- a/results/excel/accuracy_score.xlsx
+++ b/results/excel/accuracy_score.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Classification results: accuracy score</t>
   </si>
@@ -25,7 +25,7 @@
     <t>General information about the classification software</t>
   </si>
   <si>
-    <t>Issue date: 07/02/2021 10:42:22</t>
+    <t>Issue date: 18/03/2021 14:47:48</t>
   </si>
   <si>
     <t>Python version: Python 3.8.5</t>
@@ -55,7 +55,7 @@
     <t>Results:</t>
   </si>
   <si>
-    <t>Hebrew</t>
+    <t>english</t>
   </si>
   <si>
     <t>TF-IDF: 1000 words unigrams</t>
@@ -64,37 +64,10 @@
     <t>None</t>
   </si>
   <si>
-    <t>33% train test split</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>TF-IDF: 2000 words unigrams</t>
-  </si>
-  <si>
-    <t>TF-IDF: 3000 words unigrams</t>
-  </si>
-  <si>
-    <t>TF-IDF: 4000 words unigrams</t>
-  </si>
-  <si>
-    <t>TF-IDF: 5000 words unigrams</t>
-  </si>
-  <si>
-    <t>86.0</t>
-  </si>
-  <si>
-    <t>84.0</t>
-  </si>
-  <si>
-    <t>82.0</t>
-  </si>
-  <si>
-    <t>90.0</t>
-  </si>
-  <si>
-    <t>76.0</t>
+    <t>5 folds X 20 iterations CV</t>
+  </si>
+  <si>
+    <t>65.5</t>
   </si>
   <si>
     <t>Number</t>
@@ -244,8 +217,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:L25" totalsRowShown="0">
-  <autoFilter ref="A15:L25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:L16" totalsRowShown="0">
+  <autoFilter ref="A15:L16"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Number"/>
     <tableColumn id="2" name="Language"/>
@@ -260,7 +233,7 @@
     <tableColumn id="11" name="MNB"/>
     <tableColumn id="12" name="RNN"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -549,7 +522,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -559,7 +532,7 @@
     <col min="3" max="3" width="27.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -623,45 +596,45 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" t="s">
         <v>27</v>
       </c>
-      <c r="B15" t="s">
+      <c r="K15" t="s">
         <v>28</v>
       </c>
-      <c r="C15" t="s">
+      <c r="L15" t="s">
         <v>29</v>
-      </c>
-      <c r="D15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" t="s">
-        <v>35</v>
-      </c>
-      <c r="J15" t="s">
-        <v>36</v>
-      </c>
-      <c r="K15" t="s">
-        <v>37</v>
-      </c>
-      <c r="L15" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="8">
-        <v>867</v>
+        <v>0</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>13</v>
@@ -678,335 +651,8 @@
       <c r="F16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="8">
-        <v>78</v>
-      </c>
-      <c r="H16" s="8">
-        <v>82</v>
-      </c>
-      <c r="I16" s="8">
-        <v>78</v>
-      </c>
-      <c r="J16" s="8">
-        <v>86</v>
-      </c>
-      <c r="K16" s="8">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="8">
-        <v>1000</v>
-      </c>
-      <c r="B17" s="8" t="s">
+      <c r="J16" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="8">
-        <v>80</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="8">
-        <v>82</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="8">
-        <v>867</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="8">
-        <v>80</v>
-      </c>
-      <c r="H18" s="8">
-        <v>82</v>
-      </c>
-      <c r="I18" s="8">
-        <v>78</v>
-      </c>
-      <c r="J18" s="8">
-        <v>84</v>
-      </c>
-      <c r="K18" s="8">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="8">
-        <v>1242</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="8">
-        <v>86</v>
-      </c>
-      <c r="H19" s="8">
-        <v>82</v>
-      </c>
-      <c r="I19" s="8">
-        <v>82</v>
-      </c>
-      <c r="J19" s="8">
-        <v>82</v>
-      </c>
-      <c r="K19" s="8">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="8">
-        <v>867</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="8">
-        <v>78</v>
-      </c>
-      <c r="H20" s="8">
-        <v>82</v>
-      </c>
-      <c r="I20" s="8">
-        <v>78</v>
-      </c>
-      <c r="J20" s="8">
-        <v>88</v>
-      </c>
-      <c r="K20" s="8">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="8">
-        <v>1242</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="8">
-        <v>86</v>
-      </c>
-      <c r="H21" s="8">
-        <v>82</v>
-      </c>
-      <c r="I21" s="8">
-        <v>82</v>
-      </c>
-      <c r="J21" s="8">
-        <v>76</v>
-      </c>
-      <c r="K21" s="8">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="8">
-        <v>867</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="8">
-        <v>78</v>
-      </c>
-      <c r="H22" s="8">
-        <v>82</v>
-      </c>
-      <c r="I22" s="8">
-        <v>78</v>
-      </c>
-      <c r="J22" s="8">
-        <v>84</v>
-      </c>
-      <c r="K22" s="8">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="8">
-        <v>1242</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G23" s="8">
-        <v>86</v>
-      </c>
-      <c r="H23" s="8">
-        <v>82</v>
-      </c>
-      <c r="I23" s="8">
-        <v>82</v>
-      </c>
-      <c r="J23" s="8">
-        <v>84</v>
-      </c>
-      <c r="K23" s="8">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="8">
-        <v>867</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G24" s="8">
-        <v>80</v>
-      </c>
-      <c r="H24" s="8">
-        <v>82</v>
-      </c>
-      <c r="I24" s="8">
-        <v>78</v>
-      </c>
-      <c r="J24" s="8">
-        <v>88</v>
-      </c>
-      <c r="K24" s="8">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="8">
-        <v>1242</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H25" s="8">
-        <v>82</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J25" s="8">
-        <v>80</v>
-      </c>
-      <c r="K25" s="8">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Watchdog added and some small changes in RNN
</commit_message>
<xml_diff>
--- a/results/excel/accuracy_score.xlsx
+++ b/results/excel/accuracy_score.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
   <si>
     <t>Classification results: accuracy score</t>
   </si>
@@ -25,7 +25,7 @@
     <t>General information about the classification software</t>
   </si>
   <si>
-    <t>Issue date: 01/04/2021 13:52:29</t>
+    <t>Issue date: 07/05/2021 17:42:28</t>
   </si>
   <si>
     <t>Python version: Python 3.7.6</t>
@@ -55,28 +55,43 @@
     <t>Results:</t>
   </si>
   <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>TF: 10 words unigrams</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>5 folds X 1 iterations CV</t>
+  </si>
+  <si>
+    <t>66.5*</t>
+  </si>
+  <si>
+    <t>68.0*</t>
+  </si>
+  <si>
     <t>english</t>
   </si>
   <si>
-    <t>TF-IDF: 100 words unigrams</t>
-  </si>
-  <si>
-    <t>None</t>
+    <t>Doc2VecTransfomer</t>
   </si>
   <si>
     <t>5 folds X 20 iterations CV</t>
   </si>
   <si>
-    <t>86.13</t>
-  </si>
-  <si>
-    <t>86.73</t>
-  </si>
-  <si>
-    <t>TF-IDF: 1000 words unigrams</t>
-  </si>
-  <si>
-    <t>81.92</t>
+    <t>50.0*</t>
+  </si>
+  <si>
+    <t>76.98</t>
+  </si>
+  <si>
+    <t>hebrew</t>
+  </si>
+  <si>
+    <t>67.48*</t>
   </si>
   <si>
     <t>Number</t>
@@ -226,8 +241,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:L18" totalsRowShown="0">
-  <autoFilter ref="A15:L18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:L21" totalsRowShown="0">
+  <autoFilter ref="A15:L21"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Number"/>
     <tableColumn id="2" name="Language"/>
@@ -242,7 +257,7 @@
     <tableColumn id="11" name="MNB"/>
     <tableColumn id="12" name="RNN"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -531,14 +546,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="26.7109375" customWidth="1"/>
@@ -605,45 +620,45 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F15" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G15" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="H15" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="I15" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="J15" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="K15" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="L15" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="8">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>13</v>
@@ -660,13 +675,13 @@
       <c r="F16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="G16" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="8">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>13</v>
@@ -683,7 +698,7 @@
       <c r="F17" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="G17" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -692,22 +707,91 @@
         <v>0</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="8">
+        <v>0</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L18" s="5" t="s">
+      <c r="C19" s="8" t="s">
         <v>20</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="8">
+        <v>0</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="8">
+        <v>0</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small bugs fixed, features selection now works properly
</commit_message>
<xml_diff>
--- a/results/excel/accuracy_score.xlsx
+++ b/results/excel/accuracy_score.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Classification results: accuracy score</t>
   </si>
@@ -25,7 +25,7 @@
     <t>General information about the classification software</t>
   </si>
   <si>
-    <t>Issue date: 07/05/2021 17:42:28</t>
+    <t>Issue date: 25/05/2021 11:43:27</t>
   </si>
   <si>
     <t>Python version: Python 3.7.6</t>
@@ -58,40 +58,19 @@
     <t>English</t>
   </si>
   <si>
-    <t>TF: 10 words unigrams</t>
-  </si>
-  <si>
-    <t>None</t>
+    <t>Stylistic Features: sxf</t>
+  </si>
+  <si>
+    <t>30 chi2</t>
+  </si>
+  <si>
+    <t>lowercase</t>
   </si>
   <si>
     <t>5 folds X 1 iterations CV</t>
   </si>
   <si>
-    <t>66.5*</t>
-  </si>
-  <si>
-    <t>68.0*</t>
-  </si>
-  <si>
-    <t>english</t>
-  </si>
-  <si>
-    <t>Doc2VecTransfomer</t>
-  </si>
-  <si>
-    <t>5 folds X 20 iterations CV</t>
-  </si>
-  <si>
-    <t>50.0*</t>
-  </si>
-  <si>
-    <t>76.98</t>
-  </si>
-  <si>
-    <t>hebrew</t>
-  </si>
-  <si>
-    <t>67.48*</t>
+    <t>57.5*</t>
   </si>
   <si>
     <t>Number</t>
@@ -241,8 +220,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:L21" totalsRowShown="0">
-  <autoFilter ref="A15:L21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:L16" totalsRowShown="0">
+  <autoFilter ref="A15:L16"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Number"/>
     <tableColumn id="2" name="Language"/>
@@ -257,7 +236,7 @@
     <tableColumn id="11" name="MNB"/>
     <tableColumn id="12" name="RNN"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -546,17 +525,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -620,45 +599,45 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" t="s">
         <v>26</v>
       </c>
-      <c r="B15" t="s">
+      <c r="I15" t="s">
         <v>27</v>
       </c>
-      <c r="C15" t="s">
+      <c r="J15" t="s">
         <v>28</v>
       </c>
-      <c r="D15" t="s">
+      <c r="K15" t="s">
         <v>29</v>
       </c>
-      <c r="E15" t="s">
+      <c r="L15" t="s">
         <v>30</v>
-      </c>
-      <c r="F15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" t="s">
-        <v>33</v>
-      </c>
-      <c r="I15" t="s">
-        <v>34</v>
-      </c>
-      <c r="J15" t="s">
-        <v>35</v>
-      </c>
-      <c r="K15" t="s">
-        <v>36</v>
-      </c>
-      <c r="L15" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="8">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>13</v>
@@ -670,128 +649,13 @@
         <v>15</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="8">
-        <v>10</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="J16" s="6" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="8">
-        <v>0</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L18" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="8">
-        <v>0</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="8">
-        <v>0</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L20" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="8">
-        <v>0</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PTSD HK dataset changed
</commit_message>
<xml_diff>
--- a/results/excel/accuracy_score.xlsx
+++ b/results/excel/accuracy_score.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>Classification results: accuracy score</t>
   </si>
@@ -25,7 +25,7 @@
     <t>General information about the classification software</t>
   </si>
   <si>
-    <t>Issue date: 25/05/2021 11:43:27</t>
+    <t>Issue date: 22/06/2021 11:46:03</t>
   </si>
   <si>
     <t>Python version: Python 3.7.6</t>
@@ -58,19 +58,28 @@
     <t>English</t>
   </si>
   <si>
-    <t>Stylistic Features: sxf</t>
-  </si>
-  <si>
-    <t>30 chi2</t>
+    <t>Stylistic Features: slf, frc, e50te, agf, sxf, caf, anf, spe, nw, pnf, vof, acf, inf, aof, pw, thf</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
   <si>
     <t>lowercase</t>
   </si>
   <si>
-    <t>5 folds X 1 iterations CV</t>
-  </si>
-  <si>
-    <t>57.5*</t>
+    <t>5 folds X 20 iterations CV</t>
+  </si>
+  <si>
+    <t>91.73</t>
+  </si>
+  <si>
+    <t>Hebrew</t>
+  </si>
+  <si>
+    <t>Stylistic Features: vof, huf, aof, pnf, anf, agf, frc, mef, acf, fdf</t>
+  </si>
+  <si>
+    <t>90.38V</t>
   </si>
   <si>
     <t>Number</t>
@@ -220,8 +229,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:L16" totalsRowShown="0">
-  <autoFilter ref="A15:L16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:L17" totalsRowShown="0">
+  <autoFilter ref="A15:L17"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Number"/>
     <tableColumn id="2" name="Language"/>
@@ -236,7 +245,7 @@
     <tableColumn id="11" name="MNB"/>
     <tableColumn id="12" name="RNN"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -525,17 +534,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="98.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -599,45 +608,45 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H15" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I15" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="J15" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="K15" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="L15" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="8">
-        <v>35</v>
+        <v>669</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>13</v>
@@ -656,6 +665,29 @@
       </c>
       <c r="J16" s="6" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="8">
+        <v>501</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Measuring running times and sending an email in case of an exception
</commit_message>
<xml_diff>
--- a/results/excel/accuracy_score.xlsx
+++ b/results/excel/accuracy_score.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="67">
   <si>
     <t>Classification results: accuracy score</t>
   </si>
@@ -25,10 +25,10 @@
     <t>General information about the classification software</t>
   </si>
   <si>
-    <t>Issue date: 22/06/2021 11:46:03</t>
-  </si>
-  <si>
-    <t>Python version: Python 3.7.6</t>
+    <t>Issue date: 22/07/2021 10:18:20</t>
+  </si>
+  <si>
+    <t>Python version: Python 3.8.5</t>
   </si>
   <si>
     <t>Python classification libraries: keras, sklearn, tensorflow, VADAR from nltk, WordCloud</t>
@@ -55,31 +55,130 @@
     <t>Results:</t>
   </si>
   <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Stylistic Features: slf, frc, e50te, agf, sxf, caf, anf, spe, nw, pnf, vof, acf, inf, aof, pw, thf</t>
+    <t>Hebrew</t>
+  </si>
+  <si>
+    <t>TF-IDF: 100 words unigrams</t>
   </si>
   <si>
     <t>None</t>
   </si>
   <si>
-    <t>lowercase</t>
-  </si>
-  <si>
     <t>5 folds X 20 iterations CV</t>
   </si>
   <si>
-    <t>91.73</t>
-  </si>
-  <si>
-    <t>Hebrew</t>
-  </si>
-  <si>
-    <t>Stylistic Features: vof, huf, aof, pnf, anf, agf, frc, mef, acf, fdf</t>
-  </si>
-  <si>
-    <t>90.38V</t>
+    <t>62.57*</t>
+  </si>
+  <si>
+    <t>65.33*</t>
+  </si>
+  <si>
+    <t>69.33*</t>
+  </si>
+  <si>
+    <t>73.8</t>
+  </si>
+  <si>
+    <t>70.67</t>
+  </si>
+  <si>
+    <t>TF-IDF: 1000 words unigrams</t>
+  </si>
+  <si>
+    <t>70.47</t>
+  </si>
+  <si>
+    <t>74.67</t>
+  </si>
+  <si>
+    <t>74.0</t>
+  </si>
+  <si>
+    <t>75.87</t>
+  </si>
+  <si>
+    <t>72.67</t>
+  </si>
+  <si>
+    <t>TF-IDF: 1500 words unigrams</t>
+  </si>
+  <si>
+    <t>71.77</t>
+  </si>
+  <si>
+    <t>75.33</t>
+  </si>
+  <si>
+    <t>76.1</t>
+  </si>
+  <si>
+    <t>TF-IDF: 2000 words unigrams</t>
+  </si>
+  <si>
+    <t>70.5</t>
+  </si>
+  <si>
+    <t>75.53</t>
+  </si>
+  <si>
+    <t>TF-IDF: 2500 words unigrams</t>
+  </si>
+  <si>
+    <t>70.93</t>
+  </si>
+  <si>
+    <t>TF-IDF: 3000 words unigrams</t>
+  </si>
+  <si>
+    <t>71.03</t>
+  </si>
+  <si>
+    <t>76.43</t>
+  </si>
+  <si>
+    <t>TF-IDF: 3500 words unigrams</t>
+  </si>
+  <si>
+    <t>71.33</t>
+  </si>
+  <si>
+    <t>75.9</t>
+  </si>
+  <si>
+    <t>TF-IDF: 4000 words unigrams</t>
+  </si>
+  <si>
+    <t>71.37</t>
+  </si>
+  <si>
+    <t>76.27</t>
+  </si>
+  <si>
+    <t>TF-IDF: 4500 words unigrams</t>
+  </si>
+  <si>
+    <t>71.3</t>
+  </si>
+  <si>
+    <t>76.0</t>
+  </si>
+  <si>
+    <t>TF-IDF: 500 words unigrams</t>
+  </si>
+  <si>
+    <t>68.63*</t>
+  </si>
+  <si>
+    <t>76.23</t>
+  </si>
+  <si>
+    <t>TF-IDF: 5000 words unigrams</t>
+  </si>
+  <si>
+    <t>71.13</t>
+  </si>
+  <si>
+    <t>76.87</t>
   </si>
   <si>
     <t>Number</t>
@@ -229,8 +328,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:L17" totalsRowShown="0">
-  <autoFilter ref="A15:L17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:L26" totalsRowShown="0">
+  <autoFilter ref="A15:L26"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Number"/>
     <tableColumn id="2" name="Language"/>
@@ -245,7 +344,7 @@
     <tableColumn id="11" name="MNB"/>
     <tableColumn id="12" name="RNN"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -534,14 +633,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="98.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="26.7109375" customWidth="1"/>
@@ -608,45 +707,45 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="F15" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="G15" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="H15" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="I15" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="J15" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="K15" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="L15" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="8">
-        <v>669</v>
+        <v>100</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>13</v>
@@ -658,36 +757,375 @@
         <v>15</v>
       </c>
       <c r="E16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="G16" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="H16" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="I16" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="8">
-        <v>501</v>
+        <v>1000</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>15</v>
       </c>
       <c r="E17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>17</v>
+      <c r="G17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="8">
+        <v>1500</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="8">
+        <v>2000</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="8">
+        <v>2182</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="8">
+        <v>2182</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="8">
+        <v>2182</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="8">
+        <v>2182</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="8">
+        <v>2182</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="8">
+        <v>500</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="8">
+        <v>2182</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K26" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>